<commit_message>
login app id, player id,udid api test case written
</commit_message>
<xml_diff>
--- a/api/app_api/backlog/login/password_field__negative.xlsx
+++ b/api/app_api/backlog/login/password_field__negative.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\api\app_api\backlog\login\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\api\app_api\backlog\reset_password\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DBF0C4-D713-4087-A2B9-35DC036BFA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222245E7-D5D3-4CA9-9148-051FC727C4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login_password_negative" sheetId="1" r:id="rId1"/>
+    <sheet name="reset_password_negative" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -122,130 +122,34 @@
     <t>test password field with empty value</t>
   </si>
   <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST - User Signup)
-4. fill the other required field with valid credentials and goto password field
-5. test password field with empty value
-6. review the response status code.</t>
-  </si>
-  <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST - User Signup)
-4. fill the other required field with valid credentials and goto password field
-5. verify password field with invalid characters (e.g., symbols not allowed)
-6. review the response status code.</t>
-  </si>
-  <si>
     <t>verify password field with consecutive special characters</t>
-  </si>
-  <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST - User Signup)
-4. fill the other required field with valid credentials and goto password field
-5. verify password field with consecutive special characters
-6. review the response status code.</t>
   </si>
   <si>
     <t>test password field with disallowed characters specified in the API documentation</t>
   </si>
   <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST - User Signup)
-4. fill the other required field with valid credentials and goto password field
-5. test password field with disallowed characters specified in the API documentation
-6. review the response status code.</t>
-  </si>
-  <si>
     <t>verify password field with whitespace characters only</t>
-  </si>
-  <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST - User Signup)
-4. fill the other required field with valid credentials and goto password field
-5. verify password field with whitespace characters only
-6. review the response status code.</t>
   </si>
   <si>
     <t>test password field with fewer than minimum allowed characters</t>
   </si>
   <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST - User Signup)
-4. fill the other required field with valid credentials and goto password field
-5. test password field with fewer than minimum allowed characters
-6. review the response status code.</t>
-  </si>
-  <si>
     <t>test password field with more than maximum allowed characters</t>
-  </si>
-  <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST - User Signup)
-4. fill the other required field with valid credentials and goto password field
-5. test password field with  more than maximum allowed characters
-6. review the response status code.</t>
   </si>
   <si>
     <t>test password field with special characters only</t>
   </si>
   <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST - User Signup)
-4. fill the other required field with valid credentials and goto password field
-5. test password field with special characters only
-6. review the response status code.</t>
-  </si>
-  <si>
     <t>verify password field with numeric characters only</t>
-  </si>
-  <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST - User Signup)
-4. fill the other required field with valid credentials and goto password field
-5. verify password field with numeric characters only
-6. review the response status code.</t>
   </si>
   <si>
     <t>test password field with uppercase alphabetic characters only</t>
   </si>
   <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST - User Signup)
-4. fill the other required field with valid credentials and goto password field
-5. test password field with uppercase alphabetic characters only
-6. review the response status code.</t>
-  </si>
-  <si>
     <t>verify password field with lowercase alphabetic characters only</t>
   </si>
   <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST - User Signup)
-4. fill the other required field with valid credentials and goto password field
-5. verify password field with  lowercase alphabetic characters only
-6. review the response status code.</t>
-  </si>
-  <si>
     <t>test password field with special characters and whitespace characters</t>
-  </si>
-  <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST - User Signup)
-4. fill the other required field with valid credentials and goto password field
-5. test password field with special characters and whitespace characters
-6. review the response status code.</t>
   </si>
   <si>
     <t>verify password field with special characters and newline characters</t>
@@ -254,103 +158,199 @@
     <t>test password field with special characters and tab characters</t>
   </si>
   <si>
+    <t>verify password field with special characters and control characters</t>
+  </si>
+  <si>
+    <t>test password field with special characters and Unicode characters</t>
+  </si>
+  <si>
+    <t>verify password field with special characters and invalid characters</t>
+  </si>
+  <si>
+    <t>test password field with special characters and symbols</t>
+  </si>
+  <si>
+    <t>test password field with special characters and HTML/JavaScript code</t>
+  </si>
+  <si>
+    <t>verify password field with special characters and SQL injection code</t>
+  </si>
+  <si>
+    <t>verify password field with special characters and shell injection code</t>
+  </si>
+  <si>
+    <t>test password field with special characters and command injection code</t>
+  </si>
+  <si>
+    <t>Test Scenario: Reset Password Field (Negative)</t>
+  </si>
+  <si>
     <t>1. open the postman
 2. create or open the saved request
-3. define request(method -POST - User Signup)
+3. define request(method -POST )
+4. fill the other required field with valid credentials and goto password field
+5. test password field with empty value
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST )
+4. fill the other required field with valid credentials and goto password field
+5. verify password field with whitespace characters only
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST )
+4. fill the other required field with valid credentials and goto password field
+5. test password field with fewer than minimum allowed characters
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST )
+4. fill the other required field with valid credentials and goto password field
+5. test password field with  more than maximum allowed characters
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST )
+4. fill the other required field with valid credentials and goto password field
+5. test password field with special characters only
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST )
+4. fill the other required field with valid credentials and goto password field
+5. verify password field with numeric characters only
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST )
+4. fill the other required field with valid credentials and goto password field
+5. test password field with uppercase alphabetic characters only
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST )
+4. fill the other required field with valid credentials and goto password field
+5. verify password field with  lowercase alphabetic characters only
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST )
+4. fill the other required field with valid credentials and goto password field
+5. test password field with special characters and whitespace characters
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST )
+4. fill the other required field with valid credentials and goto password field
+5. verify password field with invalid characters (e.g., symbols not allowed)
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST )
 4. fill the other required field with valid credentials and goto password field
 5. test password field with special characters and tab characters
 6. review the response status code.</t>
   </si>
   <si>
-    <t>verify password field with special characters and control characters</t>
-  </si>
-  <si>
     <t>1. open the postman
 2. create or open the saved request
-3. define request(method -POST - User Signup)
+3. define request(method -POST )
 4. fill the other required field with valid credentials and goto password field
 5. verify password field with special characters and control characters
 6. review the response status code.</t>
   </si>
   <si>
-    <t>test password field with special characters and Unicode characters</t>
-  </si>
-  <si>
     <t>1. open the postman
 2. create or open the saved request
-3. define request(method -POST - User Signup)
+3. define request(method -POST )
 4. fill the other required field with valid credentials and goto password field
 5. test password field with special characters and Unicode characters
 6. review the response status code.</t>
   </si>
   <si>
-    <t>verify password field with special characters and invalid characters</t>
-  </si>
-  <si>
     <t>1. open the postman
 2. create or open the saved request
-3. define request(method -POST - User Signup)
+3. define request(method -POST )
 4. fill the other required field with valid credentials and goto password field
 5. verify password field with special characters and invalid characters
 6. review the response status code.</t>
   </si>
   <si>
-    <t>test password field with special characters and symbols</t>
-  </si>
-  <si>
     <t>1. open the postman
 2. create or open the saved request
-3. define request(method -POST - User Signup)
+3. define request(method -POST )
 4. fill the other required field with valid credentials and goto password field
 5. test password field with special characters and symbols
 6. review the response status code.</t>
   </si>
   <si>
-    <t>test password field with special characters and HTML/JavaScript code</t>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST )
+4. fill the other required field with valid credentials and goto password field
+5. verify password field with consecutive special characters
+6. review the response status code.</t>
   </si>
   <si>
     <t>1. open the postman
 2. create or open the saved request
-3. define request(method -POST - User Signup)
+3. define request(method -POST )
 4. fill the other required field with valid credentials and goto password field
 5. test password field with special characters and HTML/JavaScript code
 6. review the response status code.</t>
   </si>
   <si>
-    <t>verify password field with special characters and SQL injection code</t>
-  </si>
-  <si>
     <t>1. open the postman
 2. create or open the saved request
-3. define request(method -POST - User Signup)
+3. define request(method -POST )
 4. fill the other required field with valid credentials and goto password field
 5. verify password field with special characters and SQL injection code
 6. review the response status code.</t>
   </si>
   <si>
-    <t>verify password field with special characters and shell injection code</t>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST )
+4. fill the other required field with valid credentials and goto password field
+5. test password field with disallowed characters specified in the API documentation
+6. review the response status code.</t>
   </si>
   <si>
     <t>1. open the postman
 2. create or open the saved request
-3. define request(method -POST - User Signup)
+3. define request(method -POST )
 4. fill the other required field with valid credentials and goto password field
 5. verify password field with special characters and shell injection code
 6. review the response status code.</t>
   </si>
   <si>
-    <t>test password field with special characters and command injection code</t>
-  </si>
-  <si>
     <t>1. open the postman
 2. create or open the saved request
-3. define request(method -POST - User Signup)
+3. define request(method -POST )
 4. fill the other required field with valid credentials and goto password field
 5. test password field with special characters and command injection code
 6. review the response status code.</t>
-  </si>
-  <si>
-    <t>Test Scenario: Login Password Field (Negative)</t>
   </si>
 </sst>
 </file>
@@ -627,7 +627,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -635,8 +639,41 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -680,12 +717,51 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -693,6 +769,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -754,11 +831,9 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -771,17 +846,11 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -789,7 +858,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -841,23 +909,19 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -870,6 +934,8 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -901,39 +967,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -942,39 +975,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1537,13 +1537,13 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G7" totalsRowCount="1" headerRowDxfId="16" dataDxfId="15" totalsRowDxfId="14">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" totalsRowLabel="SYM-API-SP-004" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" totalsRowLabel="1. needs to have postman install_x000a_2. needs to have proper defination in the documentation" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" totalsRowLabel="test password field with more than maximum allowed characters" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" totalsRowLabel="1. open the postman_x000a_2. create or open the saved request_x000a_3. define request(method -POST - User Signup)_x000a_4. fill the other required field with valid credentials and goto password field_x000a_5. test password field with  more than maximum allowed characters_x000a_6. review the response status code." dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result:" totalsRowLabel="post request should return an error response with status code 400" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" totalsRowLabel="N/A" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" totalsRowLabel="SYM-API-SP-004" dataDxfId="13" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" totalsRowLabel="1. needs to have postman install_x000a_2. needs to have proper defination in the documentation" dataDxfId="12" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" totalsRowLabel="test password field with more than maximum allowed characters" dataDxfId="11" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" totalsRowLabel="1. open the postman_x000a_2. create or open the saved request_x000a_3. define request(method -POST )_x000a_4. fill the other required field with valid credentials and goto password field_x000a_5. test password field with  more than maximum allowed characters_x000a_6. review the response status code." dataDxfId="10" totalsRowDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result:" totalsRowLabel="post request should return an error response with status code 400" dataDxfId="9" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" totalsRowLabel="N/A" dataDxfId="8" totalsRowDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="7" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Template-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1753,8 +1753,8 @@
   <dimension ref="A1:Z983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G2"/>
+      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1771,7 +1771,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -1880,7 +1880,7 @@
         <v>32</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>30</v>
@@ -1919,10 +1919,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>30</v>
@@ -1959,10 +1959,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>30</v>
@@ -1999,10 +1999,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>30</v>
@@ -2039,10 +2039,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>30</v>
@@ -2079,10 +2079,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>30</v>
@@ -2119,10 +2119,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>30</v>
@@ -2159,10 +2159,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>30</v>
@@ -2199,10 +2199,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>30</v>
@@ -2239,10 +2239,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>30</v>
@@ -2279,10 +2279,10 @@
         <v>9</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>30</v>
@@ -2319,10 +2319,10 @@
         <v>9</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>30</v>
@@ -2359,10 +2359,10 @@
         <v>9</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>30</v>
@@ -2399,10 +2399,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>30</v>
@@ -2439,10 +2439,10 @@
         <v>9</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>30</v>
@@ -2479,10 +2479,10 @@
         <v>9</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>30</v>
@@ -2519,10 +2519,10 @@
         <v>9</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>30</v>
@@ -2559,10 +2559,10 @@
         <v>9</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>30</v>
@@ -2599,10 +2599,10 @@
         <v>9</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>30</v>
@@ -2639,10 +2639,10 @@
         <v>9</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>30</v>
@@ -2679,10 +2679,10 @@
         <v>9</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>30</v>

</xml_diff>